<commit_message>
MetaData Screen Redesign Cases Signed-off-by: junaid.alam <junaid.alam@analytics.com.pk>
</commit_message>
<xml_diff>
--- a/BulkSiteUpload/BulkSiteTemplate.xlsx
+++ b/BulkSiteUpload/BulkSiteTemplate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2353" uniqueCount="51">
   <si>
     <t>PARENT_SITE_ID</t>
   </si>
@@ -89,6 +89,90 @@
   </si>
   <si>
     <t>Home</t>
+  </si>
+  <si>
+    <t>1180001</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>-81</t>
+  </si>
+  <si>
+    <t>Farm</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Punjab</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>TestRegion1</t>
+  </si>
+  <si>
+    <t>TestRegion2</t>
+  </si>
+  <si>
+    <t>40.71</t>
+  </si>
+  <si>
+    <t>-74.00</t>
+  </si>
+  <si>
+    <t>1189001</t>
+  </si>
+  <si>
+    <t>Lahore</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>1030001</t>
+  </si>
+  <si>
+    <t>1193001</t>
+  </si>
+  <si>
+    <t>1194001</t>
+  </si>
+  <si>
+    <t>1208001</t>
+  </si>
+  <si>
+    <t>1215001</t>
+  </si>
+  <si>
+    <t>1003001</t>
+  </si>
+  <si>
+    <t>1216001</t>
+  </si>
+  <si>
+    <t>1217001</t>
+  </si>
+  <si>
+    <t>1218001</t>
+  </si>
+  <si>
+    <t>1230001</t>
+  </si>
+  <si>
+    <t>1235001</t>
+  </si>
+  <si>
+    <t>1260001</t>
+  </si>
+  <si>
+    <t>1031001</t>
   </si>
 </sst>
 </file>
@@ -518,33 +602,60 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Access and Report Management redesign Signed-off-by: junaid.alam <junaid.alam@analytics.com.pk>
</commit_message>
<xml_diff>
--- a/BulkSiteUpload/BulkSiteTemplate.xlsx
+++ b/BulkSiteUpload/BulkSiteTemplate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2353" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2722" uniqueCount="54">
   <si>
     <t>PARENT_SITE_ID</t>
   </si>
@@ -173,6 +173,15 @@
   </si>
   <si>
     <t>1031001</t>
+  </si>
+  <si>
+    <t>1264001</t>
+  </si>
+  <si>
+    <t>1032001</t>
+  </si>
+  <si>
+    <t>1266001</t>
   </si>
 </sst>
 </file>
@@ -602,7 +611,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -631,7 +640,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Updation to testcases Signed-off-by: junaid.alam <junaid.alam@analytics.com.pk>
</commit_message>
<xml_diff>
--- a/BulkSiteUpload/BulkSiteTemplate.xlsx
+++ b/BulkSiteUpload/BulkSiteTemplate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2722" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3583" uniqueCount="61">
   <si>
     <t>PARENT_SITE_ID</t>
   </si>
@@ -182,6 +182,27 @@
   </si>
   <si>
     <t>1266001</t>
+  </si>
+  <si>
+    <t>1002001</t>
+  </si>
+  <si>
+    <t>1280001</t>
+  </si>
+  <si>
+    <t>1034001</t>
+  </si>
+  <si>
+    <t>1285001</t>
+  </si>
+  <si>
+    <t>1286001</t>
+  </si>
+  <si>
+    <t>1287001</t>
+  </si>
+  <si>
+    <t>1289001</t>
   </si>
 </sst>
 </file>
@@ -611,7 +632,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -640,7 +661,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Program Management Signed-off-by: junaid.alam <junaid.alam@analytics.com.pk>
</commit_message>
<xml_diff>
--- a/BulkSiteUpload/BulkSiteTemplate.xlsx
+++ b/BulkSiteUpload/BulkSiteTemplate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4297" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4420" uniqueCount="66">
   <si>
     <t>PARENT_SITE_ID</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>1007001</t>
+  </si>
+  <si>
+    <t>1036001</t>
   </si>
 </sst>
 </file>
@@ -644,7 +647,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -673,7 +676,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Signed-off-by: Junaid Alam <junaid.alam@apl.com.pk>
</commit_message>
<xml_diff>
--- a/BulkSiteUpload/BulkSiteTemplate.xlsx
+++ b/BulkSiteUpload/BulkSiteTemplate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="36">
   <si>
     <t>PARENT_SITE_ID</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>1042001</t>
+  </si>
+  <si>
+    <t>1407001</t>
   </si>
 </sst>
 </file>
@@ -555,7 +558,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -584,7 +587,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Flock Management updated Program Management updated CSM code updated
</commit_message>
<xml_diff>
--- a/BulkSiteUpload/BulkSiteTemplate.xlsx
+++ b/BulkSiteUpload/BulkSiteTemplate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="34">
   <si>
     <t>PARENT_SITE_ID</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>1441001</t>
+  </si>
+  <si>
+    <t>1003001</t>
+  </si>
+  <si>
+    <t>1019001</t>
   </si>
 </sst>
 </file>
@@ -546,7 +552,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -575,7 +581,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>

</xml_diff>